<commit_message>
coarse bitfield and bitfield enumeration handling implemented
</commit_message>
<xml_diff>
--- a/doc/Input-Output Mapping.xlsx
+++ b/doc/Input-Output Mapping.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="170">
   <si>
     <t>Device_T</t>
   </si>
@@ -630,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -663,6 +663,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -946,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1815,6 +1818,9 @@
       <c r="D63" s="3" t="s">
         <v>94</v>
       </c>
+      <c r="F63" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="G63" s="12" t="s">
         <v>156</v>
       </c>
@@ -1829,6 +1835,9 @@
       <c r="D64" s="3" t="s">
         <v>95</v>
       </c>
+      <c r="F64" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="G64" s="12" t="s">
         <v>157</v>
       </c>
@@ -1846,6 +1855,9 @@
       <c r="E65" s="3" t="s">
         <v>124</v>
       </c>
+      <c r="F65" s="9" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
@@ -1860,6 +1872,9 @@
       <c r="E66" s="3" t="s">
         <v>124</v>
       </c>
+      <c r="F66" s="7" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="67" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
@@ -1871,6 +1886,9 @@
       <c r="D67" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="F67" s="8" t="s">
+        <v>126</v>
+      </c>
       <c r="G67" s="12" t="s">
         <v>158</v>
       </c>
@@ -1888,6 +1906,9 @@
       <c r="E68" s="3" t="s">
         <v>118</v>
       </c>
+      <c r="F68" s="8" t="s">
+        <v>126</v>
+      </c>
       <c r="G68" s="12" t="s">
         <v>159</v>
       </c>
@@ -1905,6 +1926,9 @@
       <c r="E69" s="3" t="s">
         <v>118</v>
       </c>
+      <c r="F69" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="G69" s="12" t="s">
         <v>160</v>
       </c>
@@ -1933,6 +1957,9 @@
       <c r="D73" s="3" t="s">
         <v>99</v>
       </c>
+      <c r="F73" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="G73" s="12" t="s">
         <v>161</v>
       </c>
@@ -1944,6 +1971,7 @@
       <c r="C74" t="s">
         <v>68</v>
       </c>
+      <c r="F74" s="13"/>
       <c r="G74" s="12" t="s">
         <v>162</v>
       </c>
@@ -1958,6 +1986,9 @@
       <c r="D75" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="F75" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="G75" s="12" t="s">
         <v>163</v>
       </c>
@@ -1974,6 +2005,9 @@
       <c r="C78" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F78" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="G78" s="12" t="s">
         <v>164</v>
       </c>
@@ -1988,6 +2022,9 @@
       <c r="D79" s="3" t="s">
         <v>100</v>
       </c>
+      <c r="F79" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="G79" s="12" t="s">
         <v>165</v>
       </c>
@@ -2002,6 +2039,9 @@
       <c r="D80" s="3" t="s">
         <v>101</v>
       </c>
+      <c r="F80" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="G80" s="12" t="s">
         <v>167</v>
       </c>
@@ -2015,6 +2055,9 @@
       </c>
       <c r="D81" s="3" t="s">
         <v>103</v>
+      </c>
+      <c r="F81" s="8" t="s">
+        <v>126</v>
       </c>
       <c r="G81" s="12" t="s">
         <v>166</v>

</xml_diff>

<commit_message>
Detecting similar peripherals and grouping them together
</commit_message>
<xml_diff>
--- a/doc/Input-Output Mapping.xlsx
+++ b/doc/Input-Output Mapping.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="171">
   <si>
     <t>Device_T</t>
   </si>
@@ -355,9 +355,6 @@
   </si>
   <si>
     <t>Groups together multiple peripherals of the same type. Generates a dedicated package</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
   <si>
     <t>sub-word types defintions</t>
@@ -536,6 +533,12 @@
   </si>
   <si>
     <t>When specified, the string is being used by a graphical frontend to visualize the register. Otherwise the name element is displayed. The displayName may contain special characters and white spaces. The place holder s can be used and is replaced by the dimIndex substring</t>
+  </si>
+  <si>
+    <t>module xml: module attribute[id]</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
@@ -579,7 +582,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -610,6 +613,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -623,7 +632,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -655,6 +664,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -939,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -983,10 +995,10 @@
         <v>74</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -1000,10 +1012,10 @@
         <v>75</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1017,10 +1029,10 @@
         <v>76</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1034,13 +1046,13 @@
         <v>83</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="72" x14ac:dyDescent="0.3">
@@ -1054,13 +1066,13 @@
         <v>83</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
@@ -1071,13 +1083,13 @@
         <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
@@ -1114,10 +1126,10 @@
         <v>77</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1131,13 +1143,13 @@
         <v>84</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1151,13 +1163,13 @@
         <v>80</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="72" x14ac:dyDescent="0.3">
@@ -1171,13 +1183,13 @@
         <v>102</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1191,13 +1203,13 @@
         <v>85</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
@@ -1217,10 +1229,10 @@
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
@@ -1234,10 +1246,10 @@
         <v>78</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1251,10 +1263,10 @@
         <v>79</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1265,13 +1277,13 @@
         <v>9</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>110</v>
+        <v>169</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F26" s="9" t="s">
-        <v>142</v>
+      <c r="F26" s="13" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1285,13 +1297,13 @@
         <v>82</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F27" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="G27" s="11" t="s">
         <v>142</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1305,13 +1317,13 @@
         <v>82</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
@@ -1325,13 +1337,13 @@
         <v>81</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
@@ -1354,7 +1366,7 @@
         <v>82</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F31" s="10"/>
     </row>
@@ -1395,13 +1407,13 @@
         <v>87</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>142</v>
+        <v>113</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>170</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1415,13 +1427,13 @@
         <v>82</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>142</v>
+        <v>113</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>170</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1435,13 +1447,13 @@
         <v>82</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>142</v>
+        <v>113</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>170</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
@@ -1455,10 +1467,10 @@
         <v>82</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>142</v>
+        <v>113</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
@@ -1477,10 +1489,10 @@
         <v>108</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1494,13 +1506,13 @@
         <v>108</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -1514,11 +1526,11 @@
         <v>82</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
@@ -1532,13 +1544,13 @@
         <v>79</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -1552,13 +1564,13 @@
         <v>82</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
@@ -1572,10 +1584,10 @@
         <v>82</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1589,13 +1601,13 @@
         <v>88</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.3">
@@ -1618,13 +1630,13 @@
         <v>89</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.3">
@@ -1638,13 +1650,13 @@
         <v>90</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.3">
@@ -1667,13 +1679,13 @@
         <v>104</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.3">
@@ -1687,10 +1699,10 @@
         <v>91</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.3">
@@ -1704,10 +1716,10 @@
         <v>91</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1721,10 +1733,10 @@
         <v>91</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.3">
@@ -1738,7 +1750,7 @@
         <v>91</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F57" s="10"/>
     </row>
@@ -1753,10 +1765,10 @@
         <v>92</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1770,10 +1782,10 @@
         <v>93</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="60" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1787,10 +1799,10 @@
         <v>82</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.3">
@@ -1809,10 +1821,10 @@
         <v>94</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.3">
@@ -1826,10 +1838,10 @@
         <v>95</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.3">
@@ -1840,13 +1852,13 @@
         <v>11</v>
       </c>
       <c r="D65" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E65" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E65" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="F65" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.3">
@@ -1860,10 +1872,10 @@
         <v>96</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -1877,10 +1889,10 @@
         <v>97</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="68" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1894,13 +1906,13 @@
         <v>89</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="69" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1914,13 +1926,13 @@
         <v>90</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.3">
@@ -1948,10 +1960,10 @@
         <v>99</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="74" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -1963,7 +1975,7 @@
       </c>
       <c r="F74" s="12"/>
       <c r="G74" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="75" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1977,10 +1989,10 @@
         <v>97</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G75" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.3">
@@ -1996,10 +2008,10 @@
         <v>9</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.3">
@@ -2013,10 +2025,10 @@
         <v>100</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.3">
@@ -2030,10 +2042,10 @@
         <v>101</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G80" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="81" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2047,10 +2059,10 @@
         <v>103</v>
       </c>
       <c r="F81" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reading GroupName and AddressBlock implemented
</commit_message>
<xml_diff>
--- a/doc/Input-Output Mapping.xlsx
+++ b/doc/Input-Output Mapping.xlsx
@@ -952,7 +952,7 @@
   <dimension ref="B4:G81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1409,8 +1409,8 @@
       <c r="E36" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F36" s="13" t="s">
-        <v>170</v>
+      <c r="F36" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="G36" s="11" t="s">
         <v>145</v>
@@ -1449,8 +1449,8 @@
       <c r="E38" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F38" s="13" t="s">
-        <v>170</v>
+      <c r="F38" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="G38" s="11" t="s">
         <v>147</v>
@@ -1469,8 +1469,8 @@
       <c r="E39" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F39" s="13" t="s">
-        <v>170</v>
+      <c r="F39" s="8" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Register type grouping confirmed and tested
</commit_message>
<xml_diff>
--- a/doc/Input-Output Mapping.xlsx
+++ b/doc/Input-Output Mapping.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="170">
   <si>
     <t>Device_T</t>
   </si>
@@ -536,9 +535,6 @@
   </si>
   <si>
     <t>module xml: module attribute[id]</t>
-  </si>
-  <si>
-    <t>TBD</t>
   </si>
 </sst>
 </file>
@@ -582,7 +578,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -613,12 +609,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -632,7 +622,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -664,9 +654,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -951,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1282,8 +1269,8 @@
       <c r="E26" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F26" s="13" t="s">
-        <v>170</v>
+      <c r="F26" s="7" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1429,8 +1416,8 @@
       <c r="E37" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F37" s="13" t="s">
-        <v>170</v>
+      <c r="F37" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="G37" s="11" t="s">
         <v>146</v>

</xml_diff>